<commit_message>
fixes to green graphs
</commit_message>
<xml_diff>
--- a/shinyapp/data/generaldata.xlsx
+++ b/shinyapp/data/generaldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Downloads/2022_DSPG_Loudoun/shinyapp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F700F-E9D1-024B-83D9-10B77F4731C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020C64FE-7ADC-F24A-9905-EC172010A121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D0205454-8D78-5D48-BAC5-75DC969D8BCD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{D0205454-8D78-5D48-BAC5-75DC969D8BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,18 +45,6 @@
     <t>% EL</t>
   </si>
   <si>
-    <t>2018-19</t>
-  </si>
-  <si>
-    <t>2019-20</t>
-  </si>
-  <si>
-    <t>2020-21</t>
-  </si>
-  <si>
-    <t>2021-22</t>
-  </si>
-  <si>
     <t>IEP Status</t>
   </si>
   <si>
@@ -77,6 +64,18 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2018-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2019-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2020-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2021-2022</t>
   </si>
 </sst>
 </file>
@@ -212,7 +211,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -220,6 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +536,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -559,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -572,203 +571,203 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>8</v>
+      <c r="B11" s="11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" s="10"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="B16" s="9"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>10</v>
+      <c r="B19" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="8">
+        <v>10</v>
+      </c>
+      <c r="B20" s="7">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="9">
+        <v>11</v>
+      </c>
+      <c r="B21" s="8">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="9">
+        <v>12</v>
+      </c>
+      <c r="B22" s="8">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="9">
+        <v>13</v>
+      </c>
+      <c r="B23" s="8">
         <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="10"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="10"/>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>12</v>
+      <c r="B27" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="8">
+        <v>10</v>
+      </c>
+      <c r="B28" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="9">
+        <v>11</v>
+      </c>
+      <c r="B29" s="8">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="9">
+        <v>12</v>
+      </c>
+      <c r="B30" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="9">
+        <v>13</v>
+      </c>
+      <c r="B31" s="8">
         <v>11</v>
       </c>
     </row>

</xml_diff>